<commit_message>
created cluePlayers.txt, started a new test file called GameSetupTests and loading players is working
</commit_message>
<xml_diff>
--- a/CLUE_BOARD_colorCoded.xlsx
+++ b/CLUE_BOARD_colorCoded.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukevalentine/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F8CA258-7590-9F49-9652-E28CCAC8072C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{408C34C2-7A31-42FF-B11F-2EC64F07EE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="460" windowWidth="16000" windowHeight="15040" xr2:uid="{FFD9ABD6-7C02-4450-8EBC-7BAEEF13B37C}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="16020" windowHeight="13224" xr2:uid="{FFD9ABD6-7C02-4450-8EBC-7BAEEF13B37C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="38">
   <si>
     <t>A</t>
   </si>
@@ -129,6 +125,24 @@
   </si>
   <si>
     <t>Light Blue: test targets</t>
+  </si>
+  <si>
+    <t>dark purple: plums starting position</t>
+  </si>
+  <si>
+    <t>white: whites starting position</t>
+  </si>
+  <si>
+    <t>bright green: greens starting position</t>
+  </si>
+  <si>
+    <t>baby blue: peacock's starting position</t>
+  </si>
+  <si>
+    <t>red: scarlet's starting position</t>
+  </si>
+  <si>
+    <t>dark yellow: mustards starting position</t>
   </si>
 </sst>
 </file>
@@ -150,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +231,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,6 +330,21 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,6 +353,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CC33"/>
       <color rgb="FFAC9FFF"/>
       <color rgb="FFFF99CC"/>
       <color rgb="FF99FF66"/>
@@ -613,18 +667,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4B6445-A3FF-4CEF-AB1F-5FCDD6E64F0C}">
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -643,7 +697,7 @@
       <c r="F1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="23" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -658,7 +712,7 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="24" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -707,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -791,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -875,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -959,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1043,7 +1097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1211,7 +1265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1295,7 +1349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1379,7 +1433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1463,7 +1517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1713,7 +1767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1797,8 +1851,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1881,7 +1935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>9</v>
       </c>
@@ -1965,7 +2019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -2049,7 +2103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2133,7 +2187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2301,7 +2355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2385,7 +2439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2469,7 +2523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2553,7 +2607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -2721,7 +2775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -2734,7 +2788,7 @@
       <c r="D26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="21" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2755,7 +2809,7 @@
       <c r="K26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -2788,7 +2842,7 @@
       <c r="V26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="W26" s="5" t="s">
+      <c r="W26" s="22" t="s">
         <v>9</v>
       </c>
       <c r="X26" s="5" t="s">
@@ -2805,7 +2859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -2910,57 +2964,73 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>